<commit_message>
bobrownicka I i II
</commit_message>
<xml_diff>
--- a/Kerim_Dane_ceny_mieszkan.xlsx
+++ b/Kerim_Dane_ceny_mieszkan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5B9176-1282-4DDB-BF59-9454CDACEAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8742AD02-89B8-464E-A8ED-E32C3273D7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7368" yWindow="1500" windowWidth="23040" windowHeight="12660" xr2:uid="{336D2583-5C4C-4C42-9206-61D546232E49}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{336D2583-5C4C-4C42-9206-61D546232E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Kerim_Dane_ceny_mieszkan_18_09_" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="88">
   <si>
     <t>Nazwa dewelopera</t>
   </si>
@@ -271,6 +271,30 @@
   </si>
   <si>
     <t>2025-09-02 00:00:00</t>
+  </si>
+  <si>
+    <t>Poznań</t>
+  </si>
+  <si>
+    <t>Bobrownicka</t>
+  </si>
+  <si>
+    <t>Borownicka</t>
+  </si>
+  <si>
+    <t>61-306</t>
+  </si>
+  <si>
+    <t>2025-12-20 00:00:00</t>
+  </si>
+  <si>
+    <t>Udział w działce drogowej</t>
+  </si>
+  <si>
+    <t>https://kerimdevelopment.pl/poznan-ul-bobrownicka-i/</t>
+  </si>
+  <si>
+    <t>https://kerimdevelopment.pl/poznan-ul-bobrownicka-ii/</t>
   </si>
 </sst>
 </file>
@@ -281,10 +305,19 @@
     <numFmt numFmtId="164" formatCode="00\-000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -308,8 +341,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -317,10 +351,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA33353A-1A07-421F-B982-7CDBB172178E}">
-  <dimension ref="A1:BF3"/>
+  <dimension ref="A1:BF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BC18" sqref="BC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,22 +709,28 @@
     <col min="11" max="11" width="18.6640625" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" customWidth="1"/>
     <col min="27" max="27" width="10.88671875" customWidth="1"/>
+    <col min="28" max="28" width="9.44140625" customWidth="1"/>
+    <col min="29" max="29" width="15.21875" customWidth="1"/>
+    <col min="30" max="30" width="11.6640625" customWidth="1"/>
+    <col min="34" max="34" width="11.5546875" customWidth="1"/>
     <col min="36" max="36" width="15.77734375" customWidth="1"/>
     <col min="37" max="37" width="15.6640625" customWidth="1"/>
     <col min="38" max="38" width="21.5546875" customWidth="1"/>
     <col min="39" max="39" width="19.5546875" style="4" customWidth="1"/>
-    <col min="40" max="40" width="16.6640625" customWidth="1"/>
+    <col min="40" max="40" width="30.21875" customWidth="1"/>
     <col min="41" max="41" width="37.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="11.77734375" customWidth="1"/>
     <col min="43" max="43" width="21.109375" style="4" customWidth="1"/>
     <col min="44" max="44" width="17.6640625" customWidth="1"/>
-    <col min="45" max="45" width="11.44140625" customWidth="1"/>
-    <col min="47" max="47" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18" customWidth="1"/>
+    <col min="46" max="46" width="20.44140625" customWidth="1"/>
+    <col min="47" max="47" width="14.6640625" customWidth="1"/>
     <col min="48" max="48" width="20.109375" customWidth="1"/>
     <col min="51" max="51" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="26.6640625" customWidth="1"/>
+    <col min="52" max="52" width="8.5546875" customWidth="1"/>
+    <col min="53" max="53" width="25.5546875" customWidth="1"/>
     <col min="54" max="54" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="13.88671875" customWidth="1"/>
     <col min="56" max="56" width="13.77734375" customWidth="1"/>
@@ -880,7 +921,7 @@
       <c r="B2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1045,58 +1086,719 @@
       <c r="BE2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BF2" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="4"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
-      <c r="AV3" s="4"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="4"/>
-      <c r="AZ3" s="4"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="3"/>
-      <c r="BC3" s="4"/>
-      <c r="BD3" s="4"/>
-      <c r="BE3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5252970002</v>
+      </c>
+      <c r="F3" s="1">
+        <v>52619039300000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>502450566</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>8511.2800000000007</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN3">
+        <v>1690000</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP3">
+        <v>1690000</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5252970002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>52619039300000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>502450566</v>
+      </c>
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK4">
+        <v>2</v>
+      </c>
+      <c r="AL4">
+        <v>9037.17</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN4">
+        <v>1590000</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP4">
+        <v>1590000</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5252970002</v>
+      </c>
+      <c r="F5" s="1">
+        <v>52619039300000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>502450566</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>9387.4599999999991</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN5">
+        <v>1790000</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP5">
+        <v>1802300</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT5">
+        <v>12300</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5252970002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>52619039300000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>502450566</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK6">
+        <v>2</v>
+      </c>
+      <c r="AL6">
+        <v>9387.4599999999991</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN6">
+        <v>1790000</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP6">
+        <v>1802300</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT6">
+        <v>12300</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BF2" r:id="rId1" xr:uid="{755F2191-46C9-4F28-8CFD-E2A705B3B241}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>